<commit_message>
Add Burndown Chart and update Product Backlog
</commit_message>
<xml_diff>
--- a/Booklet/Product Backlog Labmon.xlsx
+++ b/Booklet/Product Backlog Labmon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\condr\Desktop\UNI\LAB\1850965_Labmon\Booklet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CC915B-A3BF-433D-9915-E10FB511826C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F518C637-260D-45B5-AA1B-D3C33C430288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="141">
   <si>
     <t>Story Name</t>
   </si>
@@ -385,9 +385,6 @@
     <t>Valerio Liberati</t>
   </si>
   <si>
-    <t>Added Authentication frontend and backend for both Players and Admins.</t>
-  </si>
-  <si>
     <t>Fixed Token management and inconsistencies between frontend and backend in Authentication.</t>
   </si>
   <si>
@@ -524,6 +521,18 @@
   </si>
   <si>
     <t>09/26/2025</t>
+  </si>
+  <si>
+    <t>0.1.0.2</t>
+  </si>
+  <si>
+    <t>09/20/2025</t>
+  </si>
+  <si>
+    <t>Added Authentication backend for both Players and Admins.</t>
+  </si>
+  <si>
+    <t>Added Authentication frontend for both Players and Admins.</t>
   </si>
 </sst>
 </file>
@@ -600,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -646,9 +655,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -885,7 +891,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="A1:D34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="A1:D35">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Version"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Date"/>
@@ -1219,7 +1225,7 @@
   </sheetPr>
   <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="157" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="157" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
@@ -2032,11 +2038,11 @@
     <tabColor rgb="FFB7B7B7"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2057,7 +2063,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
@@ -2065,10 +2071,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -2076,80 +2082,80 @@
     </row>
     <row r="3" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="B5" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="13" t="s">
+      <c r="B7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="15">
-        <v>45933</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>122</v>
-      </c>
       <c r="D7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B8" s="15">
-        <v>45935</v>
+        <v>45933</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>121</v>
@@ -2158,12 +2164,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B9" s="15">
-        <v>45937</v>
+        <v>45935</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>120</v>
@@ -2172,29 +2178,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="18">
-        <v>45939</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>97</v>
+        <v>105</v>
+      </c>
+      <c r="B10" s="15">
+        <v>45937</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="D10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" s="18">
-        <v>45940</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>103</v>
+        <v>122</v>
+      </c>
+      <c r="B11" s="15">
+        <v>45941</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -2202,27 +2208,27 @@
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="18">
+        <v>123</v>
+      </c>
+      <c r="B12" s="15">
         <v>45941</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>98</v>
+      <c r="C12" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" s="18">
-        <v>45941</v>
+        <v>124</v>
+      </c>
+      <c r="B13" s="15">
+        <v>45942</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -2230,13 +2236,13 @@
     </row>
     <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B14" s="18">
-        <v>45941</v>
+        <v>125</v>
+      </c>
+      <c r="B14" s="15">
+        <v>45942</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -2244,13 +2250,13 @@
     </row>
     <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="18">
+        <v>126</v>
+      </c>
+      <c r="B15" s="15">
         <v>45942</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -2258,13 +2264,13 @@
     </row>
     <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B16" s="18">
-        <v>45942</v>
+        <v>127</v>
+      </c>
+      <c r="B16" s="15">
+        <v>45943</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -2272,38 +2278,38 @@
     </row>
     <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" s="18">
-        <v>45944</v>
+        <v>128</v>
+      </c>
+      <c r="B17" s="15">
+        <v>45943</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B18" s="4">
+    <row r="18" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="15">
+        <v>45945</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="4">
         <v>45947</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="4">
-        <v>45950</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>108</v>
@@ -2314,41 +2320,41 @@
     </row>
     <row r="20" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B20" s="4">
-        <v>45951</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>114</v>
+        <v>45950</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D20">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" s="4">
+        <v>45951</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="4">
         <v>45955</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" s="4">
-        <v>45957</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>111</v>
+      <c r="C22" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D22">
         <v>7</v>
@@ -2356,22 +2362,31 @@
     </row>
     <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B23" s="4">
-        <v>45958</v>
+        <v>45957</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D23">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3"/>
+    <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="4">
+        <v>45958</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -2422,6 +2437,11 @@
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>